<commit_message>
COmpleted Rpa challange in reframework
</commit_message>
<xml_diff>
--- a/vajrang/Team6/Week1/Data/Config.xlsx
+++ b/vajrang/Team6/Week1/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/FrameworkTemplates/REFramework/VB/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uipath\GitSpace\RPA-Developer-in-30-Days\vajrang\Team6\Week1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A0796C-CF27-417F-91BC-4611FCD2133E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10248" yWindow="17508" windowWidth="21252" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
-    <t>Framework</t>
-  </si>
-  <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>Team6 W1 Rpa Challenge</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -585,22 +585,22 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -609,10 +609,10 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1620,7 +1620,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1673,18 +1673,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1708,7 +1708,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1730,7 +1730,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +1741,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,53 +1752,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2783,7 +2783,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2802,7 +2802,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>